<commit_message>
front: script para criação do front-end com streamlit
</commit_message>
<xml_diff>
--- a/data/Key Words Pesquisa automática de legislação 3.xlsx
+++ b/data/Key Words Pesquisa automática de legislação 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJECTS\File validation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3501970E-99BC-4F47-8837-1D19FA94ECD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57DA7DF-C67D-44DB-93AF-C38902A6DC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{2B4B61A9-F03B-434E-B9F3-94E1E5A6A77C}"/>
   </bookViews>
@@ -429,7 +429,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,6 +440,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -471,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -481,6 +489,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE6D3EB-FFE1-4A55-8965-B3D5A39ADFBF}">
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -807,7 +816,7 @@
     <col min="2" max="2" width="29.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -815,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -823,7 +832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -831,7 +840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -839,7 +848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -847,15 +856,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -863,7 +873,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -871,7 +881,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -879,7 +889,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -887,7 +897,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -895,7 +905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -903,7 +913,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -911,7 +921,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -919,7 +929,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>127</v>
       </c>

</xml_diff>